<commit_message>
wating for practical results
</commit_message>
<xml_diff>
--- a/times.xlsx
+++ b/times.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>Comm</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Sequencial</t>
+  </si>
+  <si>
+    <t>MPI (Ethernet)</t>
+  </si>
+  <si>
+    <t>MPI (Myrinet)</t>
   </si>
 </sst>
 </file>
@@ -360,7 +366,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2628,10 +2633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R9"/>
+  <dimension ref="A2:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,9 +2644,9 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -2659,7 +2664,7 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2706,32 +2711,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>14.370657</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>14.421497</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>14.414141000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>14.372161999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>14.37124</v>
       </c>
     </row>
-    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <f>MEDIAN(B4:B8)</f>
         <v>14.372161999999999</v>
@@ -2793,10 +2798,172 @@
         <v>#NUM!</v>
       </c>
     </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1">
+        <v>12</v>
+      </c>
+      <c r="I12" s="1">
+        <v>16</v>
+      </c>
+      <c r="J12" s="1">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>2</v>
+      </c>
+      <c r="N12" s="1">
+        <v>4</v>
+      </c>
+      <c r="O12" s="1">
+        <v>8</v>
+      </c>
+      <c r="P12" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>16</v>
+      </c>
+      <c r="R12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>14.370657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>14.421497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>14.414141000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14.372161999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14.37124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2">
+        <f>MEDIAN(B13:B17)</f>
+        <v>14.372161999999999</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="e">
+        <f t="shared" ref="D18:R18" si="1">MEDIAN(D13:D17)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E18" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F18" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G18" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H18" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="I18" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="J18" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2" t="e">
+        <f t="shared" ref="L18:R18" si="2">MEDIAN(L13:L17)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="R18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="L2:R2"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="L11:R11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2806,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working on myrinet results
</commit_message>
<xml_diff>
--- a/times.xlsx
+++ b/times.xlsx
@@ -2209,6 +2209,613 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Eth - Tempo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Times!$B$3,Times!$D$3:$J$3)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sequencial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Times!$B$9,Times!$D$9:$J$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>14.372161999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.518706999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1697160000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1350319999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9131450000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5503879999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3054700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2551379999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-34AA-4786-8718-42DE21F70D5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Eth - Com</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$K$9:$R$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25735599999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27445900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90936499999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28875000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29761100000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30529800000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.31705499999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-34AA-4786-8718-42DE21F70D5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Myr - Tempo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Times!$B$19,Times!$D$19:$G$19)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>14.372161999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.965225</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7840759999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4015129999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.572155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-34AA-4786-8718-42DE21F70D5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Myr - Com</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$K$19:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29695100000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33107599999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31273200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32095699999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-34AA-4786-8718-42DE21F70D5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="370568528"/>
+        <c:axId val="370570824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="370568528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Número</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de Processos</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370570824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="370570824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tempo (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370568528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2765,7 +3372,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-PT"/>
@@ -3534,6 +4141,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5547,7 +6194,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5751,6 +6398,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -6051,7 +7201,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6673,6 +7823,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>173565</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>72344</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7011,8 +8191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R51" sqref="R51"/>
+    <sheetView tabSelected="1" topLeftCell="C33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>